<commit_message>
Solving TLE eliminators 800 level
</commit_message>
<xml_diff>
--- a/TLE eliminators/TLE eliminators study.xlsx
+++ b/TLE eliminators/TLE eliminators study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\resources\Competitive Programming\solutions\TLE eliminators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2000D5EA-4E67-463E-AE78-2EEBA7A31D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1103C0A-6242-4327-B55A-406023881E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily practice" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="104">
   <si>
     <t>Date</t>
   </si>
@@ -445,16 +445,6 @@
     <t>If the question asks for a YES or NO as answer, then most likely you do not need to solve what is given but a find a constraint which breaks the condition for solving and return answer</t>
   </si>
   <si>
-    <t>I was trying very hard to find out a condition where if number of negative is greater than or equal to number of positives, then how many negatives to be converted to get the answer. But I was always getting stuck with one test case or another.
-Finally after hours of finding out cases, I got the solution myself (Will be checking editorial for sure)
-Cases:
-np --&gt; number of 1s
-nn --&gt; number of -1s 
-1. If np == n: return 0 (since all are positive)
-2. if np&gt;nn: return 0 if even number of -1s else return 1 (since 1s &gt; -1s, sum will always be greater than 0, we need to take care of the product and if there are even number of -1s, product will also be =ve, so returning 0, else make 1 -1 as 1, so one operation)
-3. This is the difficult part where nn&gt;=np (see code in the column aside)</t>
-  </si>
-  <si>
     <t>def solution(n,arr):
     np = 0
     nn = 0
@@ -494,6 +484,88 @@
   </si>
   <si>
     <t>19th - 20th May, 2025</t>
+  </si>
+  <si>
+    <t>I was trying very hard to find out a condition where if number of negative is greater than or equal to number of positives, then how many negatives to be converted to get the answer. But I was always getting stuck with one test case or another.
+Finally after hours of finding out cases, I got the solution myself (Will be checking editorial for sure)
+Cases:
+np --&gt; number of 1s
+nn --&gt; number of -1s 
+1. If np == n: return 0 (since all are positive)
+2. if np&gt;nn: return 0 if even number of -1s else return 1 (since 1s &gt; -1s, sum will always be greater than 0, we need to take care of the product and if there are even number of -1s, product will also be =ve, so returning 0, else make 1 -1 as 1, so one operation)
+3. This is the difficult part where nn&gt;=np (see code in the column aside)
+Here is the change of perspective from the editorial.
+Now, since this is not a YES or NO question, they went ahead and performed the operations in a loop. That makes the code much easier. Yes, my code is O(1) to find the solution but to get the number of 1s and -1s I am anyways doing a O(n) so that doesnt help !
+So, based on the solution given in the editorial, this indeed is a easy problem</t>
+  </si>
+  <si>
+    <t>Sometimes, when the question asks for a direct answer and the solution looks too mathematical, that is, a lot of equations and if-else complexities, try solving the question by doing the action itself since the action itself is very trivial. Complexity optimization takes the back bench then</t>
+  </si>
+  <si>
+    <t>20th May, 2025</t>
+  </si>
+  <si>
+    <t>Twin permutations</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/1831/A</t>
+  </si>
+  <si>
+    <t>I am thinking of how to find that permutation.
+Thought of sorting the array, failed for  1,2,4,5,3
+Though of sorting the part which was unsorted. Failed for 1,3,8,5,6,10
+Thinking of an idea, where I find the sum of max+min and then develop the array by subtracting the sum with every element. This works !</t>
+  </si>
+  <si>
+    <t>23rd May, 2025</t>
+  </si>
+  <si>
+    <t>Blank space</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/1829/B</t>
+  </si>
+  <si>
+    <t>Just keep track of the last one</t>
+  </si>
+  <si>
+    <t>Coins</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/1814/A</t>
+  </si>
+  <si>
+    <t>Easy only because I got the observation correct
+So, I had to find a way where the condition will always be false and after playing around with a few cases, it seemed that the condition will always be false if k is even but n is false
+I have later gone through the proof of why this is always true. See notes</t>
+  </si>
+  <si>
+    <t>Walking master</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/1806/A</t>
+  </si>
+  <si>
+    <t>I found out 2 things:
+1. If the point (c,d) is below the diagonal of (a,b) its not reachable. And we can find by the line equations
+2. If the line is on the diagonal then we are good by simply subtracting (x1-x2)
+But I am stuck that if its above the diagonal, how to determine ?
+I found out that you can simply find out the exact point below it and to go right above its 2*(direct distance)
+But this is not working
+I then thought hard and worked out some maths
+We need to move from (x1,y1) to (x2,y2)
+If y2 &lt; y1, we can never go with the left and diag moves
+Also, if (x2,y2) is below the diagonal. i.e, y2&lt;y1+x2-x1 then not possible.
+Now, comes the case where its possible.
+To do that we need to find a point (p,q) so that we can do k number of left moves and z number of diag moves.
+Now, if you observe carefully, for (p,q) q will always be achieved by moving left, thus q = y1
+Now p will be in the same diagonal as (x2,y2) 
+Thus, p = y1 - y2 + x2
+So, we get (p,q)
+Thus, the total distance will be abs(x1 - p) + abs(y2 - q)</t>
+  </si>
+  <si>
+    <t>Maths is essential for CF problems</t>
   </si>
 </sst>
 </file>
@@ -928,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y20"/>
+  <dimension ref="A1:Y24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1292,7 +1364,7 @@
     </row>
     <row r="20" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>81</v>
@@ -1304,10 +1376,78 @@
         <v>75</v>
       </c>
       <c r="E20" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>86</v>
+    </row>
+    <row r="21" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="345.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1366,13 +1506,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2047B5-B884-49A6-A712-BA9886E6F78A}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="255.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
@@ -1384,6 +1527,16 @@
         <v>84</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>